<commit_message>
Added benchmark for range queries to see at which point range retrieval queries reach chunk retrieval time results.
Removed binary files.
More automation for the benchmark script.
</commit_message>
<xml_diff>
--- a/analysis/Hyperdex Benchmarks.xlsx
+++ b/analysis/Hyperdex Benchmarks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Three repetitions benchmark" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="21">
   <si>
     <t>Block Size</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>Chunked &amp; Compressed &amp; Encrypted</t>
+  </si>
+  <si>
+    <t>add single x 1000</t>
+  </si>
+  <si>
+    <t>range queries to plot func</t>
+  </si>
+  <si>
+    <t>what’s the factor between single and double dimension in PUT requests?</t>
   </si>
 </sst>
 </file>
@@ -950,11 +959,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-452040544"/>
-        <c:axId val="-452037712"/>
+        <c:axId val="329186672"/>
+        <c:axId val="329189504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-452040544"/>
+        <c:axId val="329186672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -997,7 +1006,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-452037712"/>
+        <c:crossAx val="329189504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1005,7 +1014,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-452037712"/>
+        <c:axId val="329189504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.5"/>
@@ -1026,7 +1035,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1057,7 +1066,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-452040544"/>
+        <c:crossAx val="329186672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1568,11 +1577,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-486756336"/>
-        <c:axId val="-486753072"/>
+        <c:axId val="210310592"/>
+        <c:axId val="210453968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-486756336"/>
+        <c:axId val="210310592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1615,7 +1624,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-486753072"/>
+        <c:crossAx val="210453968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1623,7 +1632,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-486753072"/>
+        <c:axId val="210453968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1673,7 +1682,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-486756336"/>
+        <c:crossAx val="210310592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3174,8 +3183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD27"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="S8" zoomScale="166" zoomScaleNormal="117" workbookViewId="0">
+      <selection activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19824,7 +19833,7 @@
         <v>0.12807900000000003</v>
       </c>
       <c r="T7" s="10">
-        <f t="shared" ref="T7:T8" si="1">K7</f>
+        <f t="shared" ref="T7" si="1">K7</f>
         <v>3.645481666666667</v>
       </c>
       <c r="V7" s="10">
@@ -20095,7 +20104,7 @@
       <c r="M16" s="22"/>
       <c r="N16" s="23"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="20"/>
       <c r="B17" s="29"/>
       <c r="C17" s="21" t="s">
@@ -20127,7 +20136,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
         <v>4</v>
       </c>
@@ -20160,8 +20169,11 @@
       <c r="N18" s="23">
         <v>12.272311</v>
       </c>
+      <c r="V18" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="30"/>
       <c r="B19" s="29"/>
       <c r="C19" s="22">
@@ -20192,8 +20204,11 @@
       <c r="N19" s="23">
         <v>10.034162999999999</v>
       </c>
+      <c r="V19" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="30"/>
       <c r="B20" s="29"/>
       <c r="C20" s="22">
@@ -20225,7 +20240,7 @@
         <v>10.262423</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="31" t="s">
         <v>7</v>
       </c>
@@ -20268,7 +20283,7 @@
       </c>
       <c r="O21" s="26"/>
     </row>
-    <row r="22" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="30"/>
       <c r="B22" s="29"/>
       <c r="C22" s="22"/>
@@ -20284,7 +20299,7 @@
       <c r="M22" s="22"/>
       <c r="N22" s="23"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="20"/>
       <c r="B23" s="29"/>
       <c r="C23" s="21" t="s">
@@ -20315,8 +20330,11 @@
       <c r="N23" s="35" t="s">
         <v>3</v>
       </c>
+      <c r="V23" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
         <v>5</v>
       </c>
@@ -20350,7 +20368,7 @@
         <v>9.0378629999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="30"/>
       <c r="B25" s="29"/>
       <c r="C25" s="22">
@@ -20382,7 +20400,7 @@
         <v>10.417142999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="30"/>
       <c r="B26" s="29"/>
       <c r="C26" s="22">
@@ -20414,7 +20432,7 @@
         <v>13.674486999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="9" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" s="9" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="36" t="s">
         <v>7</v>
       </c>
@@ -20468,7 +20486,7 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="135" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>